<commit_message>
add rbt and content start date expire date & make command for send notify & save start and expire date for rbt
</commit_message>
<xml_diff>
--- a/contentexcel/content.xlsx
+++ b/contentexcel/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rbt_system_php7\contentexcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\rbt_system_php7\contentexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,12 +77,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>mohamed mahmoud:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+2020-10-22</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mohamed mahmoud:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2020-10-27</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Content Owner</t>
   </si>
@@ -100,13 +148,19 @@
   </si>
   <si>
     <t>Contract Code</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Expire Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +196,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -472,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,9 +553,12 @@
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -507,8 +577,14 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D420:D1048576">

</xml_diff>